<commit_message>
add data to calculate kpi in task
</commit_message>
<xml_diff>
--- a/output/task_kpis_output.xlsx
+++ b/output/task_kpis_output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="53">
   <si>
     <t>ID_KPI_Target</t>
   </si>
@@ -95,7 +95,7 @@
     <t>14</t>
   </si>
   <si>
-    <t>1, 3, 7, 5, 6</t>
+    <t>1, 3, 5, 6</t>
   </si>
   <si>
     <t>1</t>
@@ -110,18 +110,15 @@
     <t>2, 7, 4, 8, 5, 6</t>
   </si>
   <si>
-    <t>2, 3, 7, 4</t>
-  </si>
-  <si>
-    <t>2, 3, 7, 4, 8</t>
+    <t>1, 2, 3, 7, 4</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 7, 4, 8</t>
   </si>
   <si>
     <t>2, 13</t>
   </si>
   <si>
-    <t>1, 2, 3, 7, 4</t>
-  </si>
-  <si>
     <t>3, 13</t>
   </si>
   <si>
@@ -134,7 +131,7 @@
     <t>2, 3, 4, 9, 16, 17, 18</t>
   </si>
   <si>
-    <t>1, 2, 7, 4, 8, 5, 6</t>
+    <t>1, 2, 7, 5, 6</t>
   </si>
   <si>
     <t>7</t>
@@ -679,19 +676,19 @@
         <v>12</v>
       </c>
       <c r="J4">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K4">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L4">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M4">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N4">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O4" t="s">
         <v>12</v>
@@ -706,7 +703,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0.12679335040317538</v>
+        <v>0.1269911480916143</v>
       </c>
       <c r="T4">
         <v>0.12214285714285714</v>
@@ -747,19 +744,19 @@
         <v>12</v>
       </c>
       <c r="J5">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K5">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L5">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M5">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N5">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O5" t="s">
         <v>12</v>
@@ -768,13 +765,13 @@
         <v>1</v>
       </c>
       <c r="Q5">
-        <v>0.2219862402693036</v>
+        <v>0.2299045158448449</v>
       </c>
       <c r="R5">
-        <v>0.18514285714285714</v>
+        <v>0.2584285714285714</v>
       </c>
       <c r="S5">
-        <v>0.20544426063439922</v>
+        <v>0.20717415191469765</v>
       </c>
       <c r="T5">
         <v>0.2314285714285714</v>
@@ -815,19 +812,19 @@
         <v>12</v>
       </c>
       <c r="J6">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K6">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L6">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M6">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N6">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O6" t="s">
         <v>12</v>
@@ -842,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>0.12679335040317538</v>
+        <v>0.1269911480916143</v>
       </c>
       <c r="T6">
         <v>0.12214285714285714</v>
@@ -883,19 +880,19 @@
         <v>12</v>
       </c>
       <c r="J7">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K7">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L7">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M7">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N7">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O7" t="s">
         <v>12</v>
@@ -910,7 +907,7 @@
         <v>0</v>
       </c>
       <c r="S7">
-        <v>0.16117839324634559</v>
+        <v>0.15992959927523195</v>
       </c>
       <c r="T7">
         <v>0.1157142857142857</v>
@@ -936,7 +933,7 @@
         <v>32</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -951,43 +948,43 @@
         <v>12</v>
       </c>
       <c r="J8">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K8">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L8">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M8">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N8">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O8" t="s">
         <v>12</v>
       </c>
       <c r="P8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q8">
-        <v>0.06637926171282403</v>
+        <v>0.21051365495046687</v>
       </c>
       <c r="R8">
-        <v>0.06557142857142857</v>
+        <v>0.18899999999999997</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>0.21887859424110348</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>0.21857142857142856</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>0.1443371080139373</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>0.1425</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1004,7 +1001,7 @@
         <v>33</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -1019,28 +1016,28 @@
         <v>12</v>
       </c>
       <c r="J9">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K9">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L9">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M9">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N9">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O9" t="s">
         <v>12</v>
       </c>
       <c r="P9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q9">
-        <v>0.05011566863587541</v>
+        <v>0.06789220875719107</v>
       </c>
       <c r="R9">
         <v>0.06171428571428572</v>
@@ -1072,7 +1069,7 @@
         <v>33</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1087,43 +1084,43 @@
         <v>12</v>
       </c>
       <c r="J10">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K10">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L10">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M10">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N10">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O10" t="s">
         <v>12</v>
       </c>
       <c r="P10">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="Q10">
-        <v>0.20317713023353673</v>
+        <v>0.1130745335178615</v>
       </c>
       <c r="R10">
-        <v>0.2147142857142857</v>
+        <v>0.08742857142857142</v>
       </c>
       <c r="S10">
-        <v>0.21764990061005743</v>
+        <v>0.09702650647735259</v>
       </c>
       <c r="T10">
-        <v>0.2314285714285714</v>
+        <v>0.1157142857142857</v>
       </c>
       <c r="U10">
-        <v>0.1443371080139373</v>
+        <v>0</v>
       </c>
       <c r="V10">
-        <v>0.135</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1137,7 +1134,7 @@
         <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1155,19 +1152,19 @@
         <v>12</v>
       </c>
       <c r="J11">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K11">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L11">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M11">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N11">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O11" t="s">
         <v>12</v>
@@ -1176,22 +1173,22 @@
         <v>2</v>
       </c>
       <c r="Q11">
-        <v>0.20317713023353673</v>
+        <v>0.21051365495046687</v>
       </c>
       <c r="R11">
-        <v>0.2147142857142857</v>
+        <v>0.18899999999999997</v>
       </c>
       <c r="S11">
-        <v>0.21764990061005743</v>
+        <v>0.21887859424110348</v>
       </c>
       <c r="T11">
-        <v>0.2314285714285714</v>
+        <v>0.21857142857142856</v>
       </c>
       <c r="U11">
         <v>0.1443371080139373</v>
       </c>
       <c r="V11">
-        <v>0.135</v>
+        <v>0.1425</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1202,13 +1199,13 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E12">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1223,43 +1220,43 @@
         <v>12</v>
       </c>
       <c r="J12">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K12">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L12">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M12">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N12">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O12" t="s">
         <v>12</v>
       </c>
       <c r="P12">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q12">
-        <v>0.13832761661060472</v>
+        <v>0.2299045158448449</v>
       </c>
       <c r="R12">
-        <v>0.135</v>
+        <v>0.2584285714285714</v>
       </c>
       <c r="S12">
-        <v>0.09893409510602233</v>
+        <v>0.20717415191469765</v>
       </c>
       <c r="T12">
-        <v>0.1157142857142857</v>
+        <v>0.2314285714285714</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>0.15506184668989548</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>0.1425</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -1270,13 +1267,13 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
         <v>37</v>
       </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
       <c r="E13">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1291,37 +1288,37 @@
         <v>12</v>
       </c>
       <c r="J13">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K13">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L13">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M13">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N13">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O13" t="s">
         <v>12</v>
       </c>
       <c r="P13">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q13">
-        <v>0.13832761661060472</v>
+        <v>0.051628615680242435</v>
       </c>
       <c r="R13">
-        <v>0.135</v>
+        <v>0.06557142857142857</v>
       </c>
       <c r="S13">
-        <v>0.09893409510602233</v>
+        <v>0</v>
       </c>
       <c r="T13">
-        <v>0.1157142857142857</v>
+        <v>0</v>
       </c>
       <c r="U13">
         <v>0</v>
@@ -1338,10 +1335,10 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
         <v>39</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
       </c>
       <c r="E14">
         <v>7</v>
@@ -1359,19 +1356,19 @@
         <v>12</v>
       </c>
       <c r="J14">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K14">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L14">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M14">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N14">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O14" t="s">
         <v>12</v>
@@ -1380,13 +1377,13 @@
         <v>7</v>
       </c>
       <c r="Q14">
-        <v>0.13832761661060472</v>
+        <v>0.1130745335178615</v>
       </c>
       <c r="R14">
-        <v>0.135</v>
+        <v>0.08742857142857142</v>
       </c>
       <c r="S14">
-        <v>0.09893409510602233</v>
+        <v>0.09702650647735259</v>
       </c>
       <c r="T14">
         <v>0.1157142857142857</v>
@@ -1406,13 +1403,13 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>8</v>
@@ -1427,43 +1424,43 @@
         <v>12</v>
       </c>
       <c r="J15">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K15">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L15">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M15">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N15">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O15" t="s">
         <v>12</v>
       </c>
       <c r="P15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q15">
-        <v>0.20317713023353673</v>
+        <v>0.2299045158448449</v>
       </c>
       <c r="R15">
-        <v>0.2147142857142857</v>
+        <v>0.2584285714285714</v>
       </c>
       <c r="S15">
-        <v>0.21764990061005743</v>
+        <v>0.20717415191469765</v>
       </c>
       <c r="T15">
         <v>0.2314285714285714</v>
       </c>
       <c r="U15">
-        <v>0.1443371080139373</v>
+        <v>0.15506184668989548</v>
       </c>
       <c r="V15">
-        <v>0.135</v>
+        <v>0.1425</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -1477,10 +1474,10 @@
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <v>8</v>
@@ -1495,40 +1492,40 @@
         <v>12</v>
       </c>
       <c r="J16">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K16">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L16">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M16">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N16">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O16" t="s">
         <v>12</v>
       </c>
       <c r="P16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q16">
-        <v>0.2219862402693036</v>
+        <v>0.21051365495046687</v>
       </c>
       <c r="R16">
-        <v>0.18514285714285714</v>
+        <v>0.18899999999999997</v>
       </c>
       <c r="S16">
-        <v>0.20544426063439922</v>
+        <v>0.21887859424110348</v>
       </c>
       <c r="T16">
-        <v>0.2314285714285714</v>
+        <v>0.21857142857142856</v>
       </c>
       <c r="U16">
-        <v>0.15506184668989548</v>
+        <v>0.1443371080139373</v>
       </c>
       <c r="V16">
         <v>0.1425</v>
@@ -1542,7 +1539,7 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
@@ -1563,19 +1560,19 @@
         <v>12</v>
       </c>
       <c r="J17">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K17">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L17">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M17">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N17">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O17" t="s">
         <v>12</v>
@@ -1590,7 +1587,7 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <v>0.16117839324634559</v>
+        <v>0.15992959927523195</v>
       </c>
       <c r="T17">
         <v>0.1157142857142857</v>
@@ -1610,7 +1607,7 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
         <v>25</v>
@@ -1631,19 +1628,19 @@
         <v>12</v>
       </c>
       <c r="J18">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K18">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L18">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M18">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N18">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O18" t="s">
         <v>12</v>
@@ -1658,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>0.12679335040317538</v>
+        <v>0.1269911480916143</v>
       </c>
       <c r="T18">
         <v>0.12214285714285714</v>
@@ -1678,13 +1675,13 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
         <v>45</v>
       </c>
-      <c r="D19" t="s">
-        <v>46</v>
-      </c>
       <c r="E19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>4</v>
@@ -1699,43 +1696,43 @@
         <v>12</v>
       </c>
       <c r="J19">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K19">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L19">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M19">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N19">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O19" t="s">
         <v>12</v>
       </c>
       <c r="P19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q19">
-        <v>0.20317713023353673</v>
+        <v>0.2299045158448449</v>
       </c>
       <c r="R19">
-        <v>0.2147142857142857</v>
+        <v>0.2584285714285714</v>
       </c>
       <c r="S19">
-        <v>0.21764990061005743</v>
+        <v>0.20717415191469765</v>
       </c>
       <c r="T19">
         <v>0.2314285714285714</v>
       </c>
       <c r="U19">
-        <v>0.1443371080139373</v>
+        <v>0.15506184668989548</v>
       </c>
       <c r="V19">
-        <v>0.135</v>
+        <v>0.1425</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -1746,10 +1743,10 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
         <v>47</v>
-      </c>
-      <c r="D20" t="s">
-        <v>48</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -1767,19 +1764,19 @@
         <v>12</v>
       </c>
       <c r="J20">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K20">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L20">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M20">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N20">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O20" t="s">
         <v>12</v>
@@ -1788,7 +1785,7 @@
         <v>3</v>
       </c>
       <c r="Q20">
-        <v>0.13001408253785554</v>
+        <v>0.13698647124939328</v>
       </c>
       <c r="R20">
         <v>0.13885714285714287</v>
@@ -1814,13 +1811,13 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21">
         <v>8</v>
@@ -1835,40 +1832,40 @@
         <v>12</v>
       </c>
       <c r="J21">
-        <v>5185</v>
+        <v>5645</v>
       </c>
       <c r="K21">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
       <c r="L21">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="M21">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="N21">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="O21" t="s">
         <v>12</v>
       </c>
       <c r="P21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q21">
-        <v>0.2219862402693036</v>
+        <v>0.21051365495046687</v>
       </c>
       <c r="R21">
-        <v>0.18514285714285714</v>
+        <v>0.18899999999999997</v>
       </c>
       <c r="S21">
-        <v>0.20544426063439922</v>
+        <v>0.21887859424110348</v>
       </c>
       <c r="T21">
-        <v>0.2314285714285714</v>
+        <v>0.21857142857142856</v>
       </c>
       <c r="U21">
-        <v>0.15506184668989548</v>
+        <v>0.1443371080139373</v>
       </c>
       <c r="V21">
         <v>0.1425</v>
@@ -1912,19 +1909,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1945,7 +1942,7 @@
         <v>17</v>
       </c>
       <c r="M3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1956,13 +1953,13 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.2219862402693036</v>
+        <v>0.2299045158448449</v>
       </c>
       <c r="D4">
-        <v>0.18514285714285714</v>
+        <v>0.2584285714285714</v>
       </c>
       <c r="E4">
-        <v>0.20544426063439922</v>
+        <v>0.20717415191469765</v>
       </c>
       <c r="F4">
         <v>0.2314285714285714</v>
@@ -1977,16 +1974,16 @@
         <v>18</v>
       </c>
       <c r="J4">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="K4">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="L4">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="M4">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1997,37 +1994,37 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>0.20317713023353673</v>
+        <v>0.21051365495046687</v>
       </c>
       <c r="D5">
-        <v>0.2147142857142857</v>
+        <v>0.18899999999999997</v>
       </c>
       <c r="E5">
-        <v>0.21764990061005743</v>
+        <v>0.21887859424110348</v>
       </c>
       <c r="F5">
-        <v>0.2314285714285714</v>
+        <v>0.21857142857142856</v>
       </c>
       <c r="G5">
         <v>0.1443371080139373</v>
       </c>
       <c r="H5">
-        <v>0.135</v>
+        <v>0.1425</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
       </c>
       <c r="J5">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="K5">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="L5">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="M5">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2038,7 +2035,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0.13001408253785554</v>
+        <v>0.13698647124939328</v>
       </c>
       <c r="D6">
         <v>0.13885714285714287</v>
@@ -2059,16 +2056,16 @@
         <v>18</v>
       </c>
       <c r="J6">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="K6">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="L6">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="M6">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2079,13 +2076,13 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>0.13832761661060472</v>
+        <v>0.1130745335178615</v>
       </c>
       <c r="D7">
-        <v>0.135</v>
+        <v>0.08742857142857142</v>
       </c>
       <c r="E7">
-        <v>0.09893409510602233</v>
+        <v>0.09702650647735259</v>
       </c>
       <c r="F7">
         <v>0.1157142857142857</v>
@@ -2100,16 +2097,16 @@
         <v>18</v>
       </c>
       <c r="J7">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="K7">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="L7">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="M7">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2120,10 +2117,10 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>0.06637926171282403</v>
+        <v>0.06789220875719107</v>
       </c>
       <c r="D8">
-        <v>0.06557142857142857</v>
+        <v>0.06171428571428572</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2141,16 +2138,16 @@
         <v>18</v>
       </c>
       <c r="J8">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="K8">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="L8">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="M8">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2161,10 +2158,10 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>0.05011566863587541</v>
+        <v>0.051628615680242435</v>
       </c>
       <c r="D9">
-        <v>0.06171428571428572</v>
+        <v>0.06557142857142857</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2182,16 +2179,16 @@
         <v>18</v>
       </c>
       <c r="J9">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="K9">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="L9">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="M9">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2208,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0.12679335040317538</v>
+        <v>0.1269911480916143</v>
       </c>
       <c r="F10">
         <v>0.12214285714285714</v>
@@ -2223,16 +2220,16 @@
         <v>18</v>
       </c>
       <c r="J10">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="K10">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="L10">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="M10">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2249,7 +2246,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0.16117839324634559</v>
+        <v>0.15992959927523195</v>
       </c>
       <c r="F11">
         <v>0.1157142857142857</v>
@@ -2264,16 +2261,16 @@
         <v>18</v>
       </c>
       <c r="J11">
-        <v>0.9010000000000001</v>
+        <v>0.901</v>
       </c>
       <c r="K11">
-        <v>0.9164285714285713</v>
+        <v>0.9035714285714285</v>
       </c>
       <c r="L11">
-        <v>0.9024999999999999</v>
+        <v>0.9099999999999999</v>
       </c>
       <c r="M11">
-        <v>0.02525567660330579</v>
+        <v>0.02543585030737396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data: add asset data
</commit_message>
<xml_diff>
--- a/output/task_kpis_output.xlsx
+++ b/output/task_kpis_output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="54">
   <si>
     <t>ID_KPI_Target</t>
   </si>
@@ -110,46 +110,49 @@
     <t>2, 7, 4, 8, 5, 6</t>
   </si>
   <si>
+    <t>1, 2, 6</t>
+  </si>
+  <si>
     <t>1, 2, 3, 7, 4</t>
   </si>
   <si>
+    <t>1, 2, 3, 4, 8</t>
+  </si>
+  <si>
     <t>1, 2, 3, 7, 4, 8</t>
   </si>
   <si>
+    <t>3, 13</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 7</t>
+  </si>
+  <si>
+    <t>4, 13</t>
+  </si>
+  <si>
+    <t>1, 3, 4</t>
+  </si>
+  <si>
     <t>2, 13</t>
   </si>
   <si>
-    <t>3, 13</t>
-  </si>
-  <si>
-    <t>4, 13</t>
-  </si>
-  <si>
-    <t>1, 2, 7, 4, 8</t>
-  </si>
-  <si>
     <t>2, 3, 4, 9, 16, 17, 18</t>
   </si>
   <si>
     <t>1, 2, 7, 5, 6</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
-    <t>1, 2, 6</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>11</t>
-  </si>
-  <si>
-    <t>1, 2, 3, 7</t>
   </si>
   <si>
     <t>12</t>
@@ -570,13 +573,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="C2">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="D2">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -676,16 +679,16 @@
         <v>12</v>
       </c>
       <c r="J4">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K4">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L4">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M4">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N4">
         <v>0.9099999999999999</v>
@@ -703,13 +706,13 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0.1269911480916143</v>
+        <v>0.1284021608481878</v>
       </c>
       <c r="T4">
         <v>0.12214285714285714</v>
       </c>
       <c r="U4">
-        <v>0.23217958108964207</v>
+        <v>0.23475935421286032</v>
       </c>
       <c r="V4">
         <v>0.24</v>
@@ -744,16 +747,16 @@
         <v>12</v>
       </c>
       <c r="J5">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K5">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L5">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M5">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N5">
         <v>0.9099999999999999</v>
@@ -765,19 +768,19 @@
         <v>1</v>
       </c>
       <c r="Q5">
-        <v>0.2299045158448449</v>
+        <v>0.23991532705858876</v>
       </c>
       <c r="R5">
-        <v>0.2584285714285714</v>
+        <v>0.2507142857142857</v>
       </c>
       <c r="S5">
-        <v>0.20717415191469765</v>
+        <v>0.20947608693597206</v>
       </c>
       <c r="T5">
         <v>0.2314285714285714</v>
       </c>
       <c r="U5">
-        <v>0.15506184668989548</v>
+        <v>0.156784756097561</v>
       </c>
       <c r="V5">
         <v>0.1425</v>
@@ -812,16 +815,16 @@
         <v>12</v>
       </c>
       <c r="J6">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K6">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L6">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M6">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N6">
         <v>0.9099999999999999</v>
@@ -839,13 +842,13 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>0.1269911480916143</v>
+        <v>0.1284021608481878</v>
       </c>
       <c r="T6">
         <v>0.12214285714285714</v>
       </c>
       <c r="U6">
-        <v>0.23217958108964207</v>
+        <v>0.23475935421286032</v>
       </c>
       <c r="V6">
         <v>0.24</v>
@@ -865,7 +868,7 @@
         <v>31</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F7">
         <v>7</v>
@@ -880,16 +883,16 @@
         <v>12</v>
       </c>
       <c r="J7">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K7">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L7">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M7">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N7">
         <v>0.9099999999999999</v>
@@ -898,25 +901,25 @@
         <v>12</v>
       </c>
       <c r="P7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>0.09032945880337852</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>0.0617316995199226</v>
       </c>
       <c r="S7">
-        <v>0.15992959927523195</v>
+        <v>0.09810457877154541</v>
       </c>
       <c r="T7">
-        <v>0.1157142857142857</v>
+        <v>0.10285714285714286</v>
       </c>
       <c r="U7">
-        <v>0.2784214642065252</v>
+        <v>0</v>
       </c>
       <c r="V7">
-        <v>0.285</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -924,40 +927,40 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>32</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G8" s="1">
-        <v>45516.20833333333</v>
+        <v>45518.20833333333</v>
       </c>
       <c r="H8" s="1">
-        <v>45523.20833333333</v>
+        <v>45519.20833333333</v>
       </c>
       <c r="I8" t="s">
         <v>12</v>
       </c>
       <c r="J8">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K8">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L8">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M8">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N8">
         <v>0.9099999999999999</v>
@@ -966,22 +969,22 @@
         <v>12</v>
       </c>
       <c r="P8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q8">
-        <v>0.21051365495046687</v>
+        <v>0.23991532705858876</v>
       </c>
       <c r="R8">
-        <v>0.18899999999999997</v>
+        <v>0.2507142857142857</v>
       </c>
       <c r="S8">
-        <v>0.21887859424110348</v>
+        <v>0.20947608693597206</v>
       </c>
       <c r="T8">
-        <v>0.21857142857142856</v>
+        <v>0.2314285714285714</v>
       </c>
       <c r="U8">
-        <v>0.1443371080139373</v>
+        <v>0.156784756097561</v>
       </c>
       <c r="V8">
         <v>0.1425</v>
@@ -992,7 +995,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
@@ -1004,7 +1007,7 @@
         <v>4</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1">
         <v>45516.20833333333</v>
@@ -1016,16 +1019,16 @@
         <v>12</v>
       </c>
       <c r="J9">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K9">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L9">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M9">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N9">
         <v>0.9099999999999999</v>
@@ -1037,10 +1040,10 @@
         <v>4</v>
       </c>
       <c r="Q9">
-        <v>0.06789220875719107</v>
+        <v>0.06437626559127371</v>
       </c>
       <c r="R9">
-        <v>0.06171428571428572</v>
+        <v>0.06680385609759144</v>
       </c>
       <c r="S9">
         <v>0</v>
@@ -1060,40 +1063,40 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E10">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10" s="1">
         <v>45516.20833333333</v>
       </c>
       <c r="H10" s="1">
-        <v>45524.20833333333</v>
+        <v>45523.20833333333</v>
       </c>
       <c r="I10" t="s">
         <v>12</v>
       </c>
       <c r="J10">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K10">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L10">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M10">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N10">
         <v>0.9099999999999999</v>
@@ -1102,25 +1105,25 @@
         <v>12</v>
       </c>
       <c r="P10">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Q10">
-        <v>0.1130745335178615</v>
+        <v>0.19630318945856384</v>
       </c>
       <c r="R10">
-        <v>0.08742857142857142</v>
+        <v>0.18514285714285714</v>
       </c>
       <c r="S10">
-        <v>0.09702650647735259</v>
+        <v>0.2213105786215602</v>
       </c>
       <c r="T10">
-        <v>0.1157142857142857</v>
+        <v>0.24428571428571427</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>0.1459408536585366</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>0.1425</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1128,40 +1131,40 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" s="1">
+        <v>45516.20833333333</v>
+      </c>
+      <c r="H11" s="1">
         <v>45524.20833333333</v>
       </c>
-      <c r="H11" s="1">
-        <v>45532.20833333333</v>
-      </c>
       <c r="I11" t="s">
         <v>12</v>
       </c>
       <c r="J11">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K11">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L11">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M11">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N11">
         <v>0.9099999999999999</v>
@@ -1170,25 +1173,25 @@
         <v>12</v>
       </c>
       <c r="P11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="Q11">
-        <v>0.21051365495046687</v>
+        <v>0.057980688384974846</v>
       </c>
       <c r="R11">
-        <v>0.18899999999999997</v>
+        <v>0.08228571428571428</v>
       </c>
       <c r="S11">
-        <v>0.21887859424110348</v>
+        <v>0</v>
       </c>
       <c r="T11">
-        <v>0.21857142857142856</v>
+        <v>0</v>
       </c>
       <c r="U11">
-        <v>0.1443371080139373</v>
+        <v>0</v>
       </c>
       <c r="V11">
-        <v>0.1425</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1199,37 +1202,37 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G12" s="1">
-        <v>45532.20833333333</v>
+        <v>45523.20833333333</v>
       </c>
       <c r="H12" s="1">
-        <v>45539.20833333333</v>
+        <v>45530.20833333333</v>
       </c>
       <c r="I12" t="s">
         <v>12</v>
       </c>
       <c r="J12">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K12">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L12">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M12">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N12">
         <v>0.9099999999999999</v>
@@ -1238,25 +1241,25 @@
         <v>12</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="Q12">
-        <v>0.2299045158448449</v>
+        <v>0.09032945880337852</v>
       </c>
       <c r="R12">
-        <v>0.2584285714285714</v>
+        <v>0.0617316995199226</v>
       </c>
       <c r="S12">
-        <v>0.20717415191469765</v>
+        <v>0.09810457877154541</v>
       </c>
       <c r="T12">
-        <v>0.2314285714285714</v>
+        <v>0.10285714285714286</v>
       </c>
       <c r="U12">
-        <v>0.15506184668989548</v>
+        <v>0</v>
       </c>
       <c r="V12">
-        <v>0.1425</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -1267,37 +1270,37 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" s="1">
-        <v>45539.20833333333</v>
+        <v>45524.20833333333</v>
       </c>
       <c r="H13" s="1">
-        <v>45545.20833333333</v>
+        <v>45530.20833333333</v>
       </c>
       <c r="I13" t="s">
         <v>12</v>
       </c>
       <c r="J13">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K13">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L13">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M13">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N13">
         <v>0.9099999999999999</v>
@@ -1306,25 +1309,25 @@
         <v>12</v>
       </c>
       <c r="P13">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="Q13">
-        <v>0.051628615680242435</v>
+        <v>0.23991532705858876</v>
       </c>
       <c r="R13">
-        <v>0.06557142857142857</v>
+        <v>0.2507142857142857</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>0.20947608693597206</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>0.2314285714285714</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>0.156784756097561</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>0.1425</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1332,40 +1335,40 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E14">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F14">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G14" s="1">
-        <v>45545.20833333333</v>
+        <v>45523.20833333333</v>
       </c>
       <c r="H14" s="1">
-        <v>45551.20833333333</v>
+        <v>45531.20833333333</v>
       </c>
       <c r="I14" t="s">
         <v>12</v>
       </c>
       <c r="J14">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K14">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L14">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M14">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N14">
         <v>0.9099999999999999</v>
@@ -1374,25 +1377,25 @@
         <v>12</v>
       </c>
       <c r="P14">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Q14">
-        <v>0.1130745335178615</v>
+        <v>0.19630318945856384</v>
       </c>
       <c r="R14">
-        <v>0.08742857142857142</v>
+        <v>0.18514285714285714</v>
       </c>
       <c r="S14">
-        <v>0.09702650647735259</v>
+        <v>0.2213105786215602</v>
       </c>
       <c r="T14">
-        <v>0.1157142857142857</v>
+        <v>0.24428571428571427</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>0.1459408536585366</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>0.1425</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -1400,40 +1403,40 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G15" s="1">
+        <v>45544.20833333333</v>
+      </c>
+      <c r="H15" s="1">
         <v>45551.20833333333</v>
       </c>
-      <c r="H15" s="1">
-        <v>45558.20833333333</v>
-      </c>
       <c r="I15" t="s">
         <v>12</v>
       </c>
       <c r="J15">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K15">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L15">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M15">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N15">
         <v>0.9099999999999999</v>
@@ -1442,25 +1445,25 @@
         <v>12</v>
       </c>
       <c r="P15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q15">
-        <v>0.2299045158448449</v>
+        <v>0</v>
       </c>
       <c r="R15">
-        <v>0.2584285714285714</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>0.20717415191469765</v>
+        <v>0.1284021608481878</v>
       </c>
       <c r="T15">
-        <v>0.2314285714285714</v>
+        <v>0.12214285714285714</v>
       </c>
       <c r="U15">
-        <v>0.15506184668989548</v>
+        <v>0.23475935421286032</v>
       </c>
       <c r="V15">
-        <v>0.1425</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -1468,40 +1471,40 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G16" s="1">
-        <v>45558.20833333333</v>
+        <v>45551.20833333333</v>
       </c>
       <c r="H16" s="1">
-        <v>45559.20833333333</v>
+        <v>45552.20833333333</v>
       </c>
       <c r="I16" t="s">
         <v>12</v>
       </c>
       <c r="J16">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K16">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L16">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M16">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N16">
         <v>0.9099999999999999</v>
@@ -1510,25 +1513,25 @@
         <v>12</v>
       </c>
       <c r="P16">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Q16">
-        <v>0.21051365495046687</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>0.18899999999999997</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>0.21887859424110348</v>
+        <v>0.16170659482273456</v>
       </c>
       <c r="T16">
-        <v>0.21857142857142856</v>
+        <v>0.1157142857142857</v>
       </c>
       <c r="U16">
-        <v>0.1443371080139373</v>
+        <v>0.2815150360310421</v>
       </c>
       <c r="V16">
-        <v>0.1425</v>
+        <v>0.285</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -1536,40 +1539,40 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G17" s="1">
+        <v>45551.20833333333</v>
+      </c>
+      <c r="H17" s="1">
         <v>45558.20833333333</v>
       </c>
-      <c r="H17" s="1">
-        <v>45560.20833333333</v>
-      </c>
       <c r="I17" t="s">
         <v>12</v>
       </c>
       <c r="J17">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K17">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L17">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M17">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N17">
         <v>0.9099999999999999</v>
@@ -1578,25 +1581,25 @@
         <v>12</v>
       </c>
       <c r="P17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>0.19630318945856384</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>0.18514285714285714</v>
       </c>
       <c r="S17">
-        <v>0.15992959927523195</v>
+        <v>0.2213105786215602</v>
       </c>
       <c r="T17">
-        <v>0.1157142857142857</v>
+        <v>0.24428571428571427</v>
       </c>
       <c r="U17">
-        <v>0.2784214642065252</v>
+        <v>0.1459408536585366</v>
       </c>
       <c r="V17">
-        <v>0.285</v>
+        <v>0.1425</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -1604,22 +1607,22 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
         <v>25</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F18">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G18" s="1">
-        <v>45559.20833333333</v>
+        <v>45558.20833333333</v>
       </c>
       <c r="H18" s="1">
         <v>45560.20833333333</v>
@@ -1628,16 +1631,16 @@
         <v>12</v>
       </c>
       <c r="J18">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K18">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L18">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M18">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N18">
         <v>0.9099999999999999</v>
@@ -1646,7 +1649,7 @@
         <v>12</v>
       </c>
       <c r="P18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -1655,16 +1658,16 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>0.1269911480916143</v>
+        <v>0.16170659482273456</v>
       </c>
       <c r="T18">
-        <v>0.12214285714285714</v>
+        <v>0.1157142857142857</v>
       </c>
       <c r="U18">
-        <v>0.23217958108964207</v>
+        <v>0.2815150360310421</v>
       </c>
       <c r="V18">
-        <v>0.24</v>
+        <v>0.285</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -1675,16 +1678,16 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G19" s="1">
         <v>45560.20833333333</v>
@@ -1696,16 +1699,16 @@
         <v>12</v>
       </c>
       <c r="J19">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K19">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L19">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M19">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N19">
         <v>0.9099999999999999</v>
@@ -1714,22 +1717,22 @@
         <v>12</v>
       </c>
       <c r="P19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q19">
-        <v>0.2299045158448449</v>
+        <v>0.19630318945856384</v>
       </c>
       <c r="R19">
-        <v>0.2584285714285714</v>
+        <v>0.18514285714285714</v>
       </c>
       <c r="S19">
-        <v>0.20717415191469765</v>
+        <v>0.2213105786215602</v>
       </c>
       <c r="T19">
-        <v>0.2314285714285714</v>
+        <v>0.24428571428571427</v>
       </c>
       <c r="U19">
-        <v>0.15506184668989548</v>
+        <v>0.1459408536585366</v>
       </c>
       <c r="V19">
         <v>0.1425</v>
@@ -1743,16 +1746,16 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E20">
         <v>3</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G20" s="1">
         <v>45565.20833333333</v>
@@ -1764,16 +1767,16 @@
         <v>12</v>
       </c>
       <c r="J20">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K20">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L20">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M20">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N20">
         <v>0.9099999999999999</v>
@@ -1785,7 +1788,7 @@
         <v>3</v>
       </c>
       <c r="Q20">
-        <v>0.13698647124939328</v>
+        <v>0.14309507070322033</v>
       </c>
       <c r="R20">
         <v>0.13885714285714287</v>
@@ -1811,13 +1814,13 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21">
         <v>8</v>
@@ -1832,16 +1835,16 @@
         <v>12</v>
       </c>
       <c r="J21">
-        <v>5645</v>
+        <v>5502</v>
       </c>
       <c r="K21">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
       <c r="L21">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="M21">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="N21">
         <v>0.9099999999999999</v>
@@ -1850,22 +1853,22 @@
         <v>12</v>
       </c>
       <c r="P21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q21">
-        <v>0.21051365495046687</v>
+        <v>0.23991532705858876</v>
       </c>
       <c r="R21">
-        <v>0.18899999999999997</v>
+        <v>0.2507142857142857</v>
       </c>
       <c r="S21">
-        <v>0.21887859424110348</v>
+        <v>0.20947608693597206</v>
       </c>
       <c r="T21">
-        <v>0.21857142857142856</v>
+        <v>0.2314285714285714</v>
       </c>
       <c r="U21">
-        <v>0.1443371080139373</v>
+        <v>0.156784756097561</v>
       </c>
       <c r="V21">
         <v>0.1425</v>
@@ -1895,13 +1898,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="B2">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="C2">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1909,19 +1912,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1942,7 +1945,7 @@
         <v>17</v>
       </c>
       <c r="M3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1953,19 +1956,19 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.2299045158448449</v>
+        <v>0.23991532705858876</v>
       </c>
       <c r="D4">
-        <v>0.2584285714285714</v>
+        <v>0.2507142857142857</v>
       </c>
       <c r="E4">
-        <v>0.20717415191469765</v>
+        <v>0.20947608693597206</v>
       </c>
       <c r="F4">
         <v>0.2314285714285714</v>
       </c>
       <c r="G4">
-        <v>0.15506184668989548</v>
+        <v>0.156784756097561</v>
       </c>
       <c r="H4">
         <v>0.1425</v>
@@ -1974,16 +1977,16 @@
         <v>18</v>
       </c>
       <c r="J4">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="K4">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="L4">
         <v>0.9099999999999999</v>
       </c>
       <c r="M4">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1994,19 +1997,19 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>0.21051365495046687</v>
+        <v>0.19630318945856384</v>
       </c>
       <c r="D5">
-        <v>0.18899999999999997</v>
+        <v>0.18514285714285714</v>
       </c>
       <c r="E5">
-        <v>0.21887859424110348</v>
+        <v>0.2213105786215602</v>
       </c>
       <c r="F5">
-        <v>0.21857142857142856</v>
+        <v>0.24428571428571427</v>
       </c>
       <c r="G5">
-        <v>0.1443371080139373</v>
+        <v>0.1459408536585366</v>
       </c>
       <c r="H5">
         <v>0.1425</v>
@@ -2015,16 +2018,16 @@
         <v>18</v>
       </c>
       <c r="J5">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="K5">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="L5">
         <v>0.9099999999999999</v>
       </c>
       <c r="M5">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2035,7 +2038,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0.13698647124939328</v>
+        <v>0.14309507070322033</v>
       </c>
       <c r="D6">
         <v>0.13885714285714287</v>
@@ -2056,16 +2059,16 @@
         <v>18</v>
       </c>
       <c r="J6">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="K6">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="L6">
         <v>0.9099999999999999</v>
       </c>
       <c r="M6">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2076,16 +2079,16 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>0.1130745335178615</v>
+        <v>0.09032945880337852</v>
       </c>
       <c r="D7">
-        <v>0.08742857142857142</v>
+        <v>0.0617316995199226</v>
       </c>
       <c r="E7">
-        <v>0.09702650647735259</v>
+        <v>0.09810457877154541</v>
       </c>
       <c r="F7">
-        <v>0.1157142857142857</v>
+        <v>0.10285714285714286</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -2097,16 +2100,16 @@
         <v>18</v>
       </c>
       <c r="J7">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="K7">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="L7">
         <v>0.9099999999999999</v>
       </c>
       <c r="M7">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2117,10 +2120,10 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>0.06789220875719107</v>
+        <v>0.06437626559127371</v>
       </c>
       <c r="D8">
-        <v>0.06171428571428572</v>
+        <v>0.06680385609759144</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2138,16 +2141,16 @@
         <v>18</v>
       </c>
       <c r="J8">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="K8">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="L8">
         <v>0.9099999999999999</v>
       </c>
       <c r="M8">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2158,10 +2161,10 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>0.051628615680242435</v>
+        <v>0.057980688384974846</v>
       </c>
       <c r="D9">
-        <v>0.06557142857142857</v>
+        <v>0.08228571428571428</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2179,16 +2182,16 @@
         <v>18</v>
       </c>
       <c r="J9">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="K9">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="L9">
         <v>0.9099999999999999</v>
       </c>
       <c r="M9">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2205,13 +2208,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0.1269911480916143</v>
+        <v>0.1284021608481878</v>
       </c>
       <c r="F10">
         <v>0.12214285714285714</v>
       </c>
       <c r="G10">
-        <v>0.23217958108964207</v>
+        <v>0.23475935421286032</v>
       </c>
       <c r="H10">
         <v>0.24</v>
@@ -2220,16 +2223,16 @@
         <v>18</v>
       </c>
       <c r="J10">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="K10">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="L10">
         <v>0.9099999999999999</v>
       </c>
       <c r="M10">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2246,13 +2249,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0.15992959927523195</v>
+        <v>0.16170659482273456</v>
       </c>
       <c r="F11">
         <v>0.1157142857142857</v>
       </c>
       <c r="G11">
-        <v>0.2784214642065252</v>
+        <v>0.2815150360310421</v>
       </c>
       <c r="H11">
         <v>0.285</v>
@@ -2261,16 +2264,16 @@
         <v>18</v>
       </c>
       <c r="J11">
-        <v>0.901</v>
+        <v>0.8855355556175141</v>
       </c>
       <c r="K11">
-        <v>0.9035714285714285</v>
+        <v>0.9164285714285715</v>
       </c>
       <c r="L11">
         <v>0.9099999999999999</v>
       </c>
       <c r="M11">
-        <v>0.02543585030737396</v>
+        <v>0.02486757536063395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>